<commit_message>
code cleanup and rename of newtonp.m to newton.m; code fix and cleanup of secant_method.m
</commit_message>
<xml_diff>
--- a/project1/projectverifyspreadsheet.xlsx
+++ b/project1/projectverifyspreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Math400\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D49A0141-ADA8-4DFE-873B-37A1ECEC8073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DC4E5F-B99A-4CC9-8246-829772A87881}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="2625" windowWidth="11820" windowHeight="12090" activeTab="1" xr2:uid="{2BF06C46-D7AE-4ADC-9BE5-B49EC4B92034}"/>
+    <workbookView xWindow="1665" yWindow="2625" windowWidth="21000" windowHeight="12090" activeTab="1" xr2:uid="{2BF06C46-D7AE-4ADC-9BE5-B49EC4B92034}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,10 +680,13 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="22.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
code cleanup and finalization; still need to complete 1.2, 3c, and 3d
</commit_message>
<xml_diff>
--- a/project1/projectverifyspreadsheet.xlsx
+++ b/project1/projectverifyspreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Math400\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DC4E5F-B99A-4CC9-8246-829772A87881}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9656BE5-29D2-4800-9333-494D589B5D35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="2625" windowWidth="21000" windowHeight="12090" activeTab="1" xr2:uid="{2BF06C46-D7AE-4ADC-9BE5-B49EC4B92034}"/>
   </bookViews>
@@ -680,7 +680,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,11 +715,11 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1.08</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>TANH(B3)</f>
-        <v>0.79319909708350078</v>
+        <v>0.76159415595576485</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -727,11 +727,11 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1.0900000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="C4">
         <f>TANH(B4)</f>
-        <v>0.7968781442047268</v>
+        <v>0.98367485769368002</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,15 +740,15 @@
       </c>
       <c r="B5">
         <f>B4-C4/D5</f>
-        <v>-1.0759905892675075</v>
+        <v>-3.8011007259710765</v>
       </c>
       <c r="C5">
         <f>TANH(B5)</f>
-        <v>-0.79170753090594626</v>
+        <v>-0.99900179660286481</v>
       </c>
       <c r="D5">
         <f>(C4-C3)/(B4-B3)</f>
-        <v>0.36790471212260167</v>
+        <v>0.15862907266993942</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,15 +757,15 @@
       </c>
       <c r="B6">
         <f>B5-C5/D6</f>
-        <v>3.4797145768388216E-3</v>
+        <v>-0.67658178197897456</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C28" si="0">TANH(B6)</f>
-        <v>3.4797005322991493E-3</v>
+        <v>-0.58929270189903182</v>
       </c>
       <c r="D6">
         <f>(C5-C4)/(B5-B4)</f>
-        <v>0.73342224245207788</v>
+        <v>0.31972979345309099</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,15 +774,15 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B28" si="1">B6-C6/D7</f>
-        <v>-1.2439948118223151E-3</v>
+        <v>3.8174756710800235</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>-1.2439941701191466E-3</v>
+        <v>0.99903394260170797</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D28" si="2">(C6-C5)/(B6-B5)</f>
-        <v>0.73664576839800411</v>
+        <v>0.13112709573793149</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,15 +791,15 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>3.2259473944137168E-9</v>
+        <v>0.99078007219118325</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>3.2259473944137168E-9</v>
+        <v>0.75769475233564232</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>0.99999689095123501</v>
+        <v>0.35342820181784806</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,15 +808,15 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>-1.6640715413302072E-15</v>
+        <v>-7.8837521551156264</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>-1.6640715413302072E-15</v>
+        <v>-0.99999971601865034</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>0.99999948416062645</v>
+        <v>8.5378556630199193E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,15 +825,15 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.8347917886337983</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.99312511087516708</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.1980605200740487</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -842,32 +842,32 @@
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>726.5524557858422</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.3615882566876951E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D12" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>360.60089379171973</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>2.7326020814089622E-3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -882,9 +882,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>